<commit_message>
ResourceMonitor v1.1.1 log threshold conditon added, version managing menual file added
</commit_message>
<xml_diff>
--- a/기능명세.xlsx
+++ b/기능명세.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>기능명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,6 +249,50 @@
   </si>
   <si>
     <t>Clogger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그 주기 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그 조건 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Threshold 설정 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">메모리 Threshold 설정 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDlgSetLogInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DlgSetLogThreshold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win32_PerfFormattedData_PerfProc_Process</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -256,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,14 +321,6 @@
       <color rgb="FFFA7D00"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF292929"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -371,9 +407,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -385,7 +423,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -696,10 +734,10 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -727,7 +765,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -743,13 +781,13 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
@@ -758,8 +796,8 @@
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>53</v>
+      <c r="E5" t="s">
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>52</v>
@@ -853,7 +891,7 @@
       <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -865,7 +903,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
@@ -878,7 +916,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1026,8 +1064,54 @@
         <v>57</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="A6:A10"/>

</xml_diff>

<commit_message>
Readme v2.0.0 Updated/ 기능명세 Updated
</commit_message>
<xml_diff>
--- a/기능명세.xlsx
+++ b/기능명세.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="기능" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>기능명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,22 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Win32_OperatingSystem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalVisibleMemorySize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'' - FreePhysicalMemory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Win32_OperatingSystem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>클래스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -218,24 +202,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PercentProcessorTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Win32_PerfRawData_PerfProc_Process</t>
-  </si>
-  <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IDProcess</t>
-  </si>
-  <si>
-    <t>WorkingSet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Clogger</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -280,10 +250,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Win32_PerfFormattedData_PerfProc_Process</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로세스 커밋 메모리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -296,47 +262,126 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PrivateBytes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WorkingSetPrivate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>KB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>프로세스 CPU 평균(60초) 사용률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win32_LogicalDIsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win32_LogicalDIsk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Etw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Etw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networkMap 추가 연산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerfDataOSProcessor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPerfDataPerProcess</t>
+  </si>
+  <si>
+    <t>m_table.cpuTotal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPerfDataPerProcess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>프로세스 CPU 사용률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프로세스 CPU 평균(60초) 사용률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PercentProcessorTime 평균필터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FreeSpace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Win32_LogicalDIsk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Win32_LogicalDIsk</t>
+    <t>CPerfDataOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSDataObj.totalVisibleMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSDataObj.freePhysicalMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_table.first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.meanUsageRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.usageRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.privateBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.workingSet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PerProcessDataObj.virtualBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LogicalDiskDataObj.deviceID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LogicalDiskDataObj.size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LogicalDiskDataObj.freeSpace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diskMap.first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networkMap.first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProcessDiskData.readBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProcessDiskData.writeBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProcessNetworkData.sendBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProcessNetworkData.receiveBytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -463,14 +508,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -755,20 +800,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.3984375" customWidth="1"/>
-    <col min="5" max="5" width="44.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="5" max="5" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -782,25 +827,31 @@
         <v>20</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
         <v>23</v>
@@ -812,13 +863,13 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
@@ -828,29 +879,29 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
@@ -860,13 +911,13 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -878,13 +929,13 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>25</v>
@@ -894,13 +945,13 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>22</v>
@@ -912,13 +963,13 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
@@ -928,61 +979,61 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>4</v>
       </c>
@@ -990,19 +1041,19 @@
         <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
@@ -1012,13 +1063,13 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
@@ -1028,13 +1079,13 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>5</v>
@@ -1046,13 +1097,13 @@
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="2" t="s">
@@ -1062,13 +1113,13 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="2" t="s">
@@ -1077,8 +1128,14 @@
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
@@ -1087,20 +1144,32 @@
       <c r="D20" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>10</v>
@@ -1112,13 +1181,13 @@
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
@@ -1128,13 +1197,13 @@
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
@@ -1143,8 +1212,14 @@
       <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="2" t="s">
@@ -1153,8 +1228,14 @@
       <c r="D25" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1168,54 +1249,59 @@
         <v>40</v>
       </c>
       <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" s="11" t="s">
+      <c r="E27" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B17:B20"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="A21:A25"/>
     <mergeCell ref="A2:A6"/>
@@ -1227,11 +1313,6 @@
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1247,9 +1328,9 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
ResourceMonitor v5.0.0 updated. Version_Dialog added, Set Log Path added.
</commit_message>
<xml_diff>
--- a/기능명세.xlsx
+++ b/기능명세.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>기능명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -382,6 +382,38 @@
   </si>
   <si>
     <t>ProcessNetworkData.receiveBytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로그램 제목에 Version 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version.txt 보여주기 메뉴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version_Dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일부 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일부 완료</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -477,7 +509,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -508,14 +540,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -798,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -809,11 +844,12 @@
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.375" customWidth="1"/>
-    <col min="5" max="5" width="44.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -824,34 +860,40 @@
         <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
         <v>23</v>
@@ -859,65 +901,77 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>70</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>68</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -925,33 +979,39 @@
         <v>24</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>22</v>
@@ -959,81 +1019,96 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>70</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>70</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>4</v>
       </c>
@@ -1043,49 +1118,58 @@
       <c r="C14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>5</v>
@@ -1093,83 +1177,98 @@
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>70</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>64</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>64</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>64</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>10</v>
@@ -1177,65 +1276,77 @@
       <c r="C22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>70</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>64</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>65</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>65</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1245,29 +1356,35 @@
       <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="3" t="s">
+      <c r="C27" s="12"/>
+      <c r="D27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>49</v>
@@ -1275,33 +1392,65 @@
       <c r="C28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
         <v>53</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B17:B20"/>
+  <mergeCells count="19">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="A21:A25"/>
     <mergeCell ref="A2:A6"/>
@@ -1313,6 +1462,11 @@
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>